<commit_message>
continued description D2 and D6
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haaan\Documents\Studium\Semester 6\Graphische Programmierung\Projekt\Parkassist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nahkusaidy/Documents/Repositories/Parkassist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65034F87-7CD4-4778-8AA3-DE87BB4EE58F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697D32D7-1686-1143-8DBE-8231FCAA1078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1760" windowWidth="14400" windowHeight="7360" xr2:uid="{1F98348F-F45F-A84B-9C98-4441577B2E35}"/>
+    <workbookView xWindow="4800" yWindow="1760" windowWidth="17400" windowHeight="13100" xr2:uid="{1F98348F-F45F-A84B-9C98-4441577B2E35}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -47,12 +47,6 @@
     <t>pessimistisch</t>
   </si>
   <si>
-    <t>&lt;T&gt;</t>
-  </si>
-  <si>
-    <t>sigmahoch2</t>
-  </si>
-  <si>
     <t>wirklich</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>2+2+</t>
+  </si>
+  <si>
+    <t>&lt;T&gt; (weighted mean)</t>
+  </si>
+  <si>
+    <t>sigma</t>
   </si>
 </sst>
 </file>
@@ -466,12 +466,16 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,18 +489,18 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>0.75</v>
@@ -511,13 +515,17 @@
         <f>(B2+4*C2+D2)/6</f>
         <v>1.0416666666666667</v>
       </c>
+      <c r="F2">
+        <f>(D2-B2)/6</f>
+        <v>0.125</v>
+      </c>
       <c r="G2">
         <v>0.75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.5</v>
@@ -532,13 +540,17 @@
         <f t="shared" ref="E3:E15" si="0">(B3+4*C3+D3)/6</f>
         <v>1</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F15" si="1">(D3-B3)/6</f>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G3">
         <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1.5</v>
@@ -553,13 +565,17 @@
         <f t="shared" si="0"/>
         <v>2.0833333333333335</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
       <c r="G4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -574,10 +590,14 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -592,10 +612,14 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -610,13 +634,17 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -631,13 +659,17 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="G8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1.5</v>
@@ -652,13 +684,17 @@
         <f t="shared" si="0"/>
         <v>2.4166666666666665</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
       <c r="G9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -673,13 +709,17 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -694,13 +734,17 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -715,10 +759,14 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -733,13 +781,17 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="G13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -754,10 +806,14 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>1.5</v>
@@ -772,10 +828,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E16">
         <f>SUM(E2:E15)</f>
@@ -783,7 +843,7 @@
       </c>
       <c r="F16">
         <f>SUM(F2:F14)</f>
-        <v>0</v>
+        <v>2.958333333333333</v>
       </c>
       <c r="G16">
         <f>SUM(G2:G14)</f>

</xml_diff>